<commit_message>
Fix unicode error crashing app
All words with unicode characters "ñ" had to de removed and
new words incorporated because these caused tkinter to crash. It appears
this is a known issued and won't be fixed.
</commit_message>
<xml_diff>
--- a/Stimuli/words/worksheet_3.xlsx
+++ b/Stimuli/words/worksheet_3.xlsx
@@ -1,21 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Box Sync/Research/Research Projects/Disertación/Methods/Materiales/Instrumentos/Materiales/Palabras/worksheets/spelling measure/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F48436B-0C3B-FB4D-B28F-351985562AD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="67">
   <si>
     <t>word</t>
   </si>
@@ -215,32 +220,39 @@
     <t>indiscretamente</t>
   </si>
   <si>
-    <t>puertorriqueño</t>
+    <t>agitadamente</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -252,26 +264,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -559,20 +589,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -595,1249 +621,1249 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="n">
+      <c r="B2">
         <v>21</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
         <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="n">
+      <c r="B3">
         <v>21</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
         <v>21</v>
       </c>
       <c r="G3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="n">
+      <c r="B4">
         <v>18</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="n">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
         <v>20</v>
       </c>
       <c r="G4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="n">
+      <c r="B5">
         <v>21</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
         <v>21</v>
       </c>
       <c r="G5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
-      <c r="B6" t="n">
+      <c r="B6">
         <v>21</v>
       </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>0</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
         <v>21</v>
       </c>
       <c r="G6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="n">
+      <c r="B7">
         <v>21</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>21</v>
       </c>
       <c r="G7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="n">
+      <c r="B8">
         <v>21</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" t="n">
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
         <v>21</v>
       </c>
       <c r="G8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B9" t="n">
+      <c r="B9">
         <v>21</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E9" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" t="n">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
         <v>21</v>
       </c>
       <c r="G9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B10" t="n">
+      <c r="B10">
         <v>21</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="n">
-        <v>0</v>
-      </c>
-      <c r="E10" t="n">
-        <v>0</v>
-      </c>
-      <c r="F10" t="n">
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>21</v>
       </c>
       <c r="G10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11" t="n">
+      <c r="B11">
         <v>30</v>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0</v>
-      </c>
-      <c r="F11" t="n">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
         <v>30</v>
       </c>
       <c r="G11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" t="n">
+      <c r="B12">
         <v>30</v>
       </c>
-      <c r="C12" t="n">
-        <v>0</v>
-      </c>
-      <c r="D12" t="n">
-        <v>0</v>
-      </c>
-      <c r="E12" t="n">
-        <v>0</v>
-      </c>
-      <c r="F12" t="n">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
         <v>30</v>
       </c>
       <c r="G12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" t="n">
+      <c r="B13">
         <v>30</v>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D13" t="n">
-        <v>0</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F13" t="n">
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
         <v>30</v>
       </c>
       <c r="G13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" t="n">
+      <c r="B14">
         <v>33</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
-      <c r="D14" t="n">
-        <v>0</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0</v>
-      </c>
-      <c r="F14" t="n">
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>33</v>
       </c>
       <c r="G14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B15">
         <v>30</v>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
-      <c r="D15" t="n">
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
         <v>2</v>
       </c>
-      <c r="E15" t="n">
-        <v>0</v>
-      </c>
-      <c r="F15" t="n">
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
         <v>32</v>
       </c>
       <c r="G15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16" t="n">
+      <c r="B16">
         <v>30</v>
       </c>
-      <c r="C16" t="n">
-        <v>0</v>
-      </c>
-      <c r="D16" t="n">
-        <v>0</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0</v>
-      </c>
-      <c r="F16" t="n">
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
         <v>30</v>
       </c>
       <c r="G16" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17" t="n">
+      <c r="B17">
         <v>33</v>
       </c>
-      <c r="C17" t="n">
-        <v>0</v>
-      </c>
-      <c r="D17" t="n">
-        <v>0</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0</v>
-      </c>
-      <c r="F17" t="n">
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
         <v>33</v>
       </c>
       <c r="G17" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18" t="n">
+      <c r="B18">
         <v>33</v>
       </c>
-      <c r="C18" t="n">
-        <v>0</v>
-      </c>
-      <c r="D18" t="n">
-        <v>0</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0</v>
-      </c>
-      <c r="F18" t="n">
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
         <v>33</v>
       </c>
       <c r="G18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19" t="n">
+      <c r="B19">
         <v>30</v>
       </c>
-      <c r="C19" t="n">
-        <v>0</v>
-      </c>
-      <c r="D19" t="n">
-        <v>0</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0</v>
-      </c>
-      <c r="F19" t="n">
+      <c r="C19">
+        <v>0</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
         <v>30</v>
       </c>
       <c r="G19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20" t="n">
+      <c r="B20">
         <v>18</v>
       </c>
-      <c r="C20" t="n">
-        <v>0</v>
-      </c>
-      <c r="D20" t="n">
-        <v>0</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0</v>
-      </c>
-      <c r="F20" t="n">
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
         <v>18</v>
       </c>
       <c r="G20" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="21" spans="1:7">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
-      <c r="B21" t="n">
+      <c r="B21">
         <v>12</v>
       </c>
-      <c r="C21" t="n">
-        <v>0</v>
-      </c>
-      <c r="D21" t="n">
-        <v>0</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0</v>
-      </c>
-      <c r="F21" t="n">
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>12</v>
       </c>
       <c r="G21" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:7">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
-      <c r="B22" t="n">
+      <c r="B22">
         <v>18</v>
       </c>
-      <c r="C22" t="n">
-        <v>0</v>
-      </c>
-      <c r="D22" t="n">
-        <v>0</v>
-      </c>
-      <c r="E22" t="n">
-        <v>0</v>
-      </c>
-      <c r="F22" t="n">
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
         <v>18</v>
       </c>
       <c r="G22" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
-      <c r="B23" t="n">
+      <c r="B23">
         <v>12</v>
       </c>
-      <c r="C23" t="n">
-        <v>0</v>
-      </c>
-      <c r="D23" t="n">
-        <v>0</v>
-      </c>
-      <c r="E23" t="n">
-        <v>0</v>
-      </c>
-      <c r="F23" t="n">
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
         <v>12</v>
       </c>
       <c r="G23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="1:7">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
-      <c r="B24" t="n">
+      <c r="B24">
         <v>9</v>
       </c>
-      <c r="C24" t="n">
-        <v>0</v>
-      </c>
-      <c r="D24" t="n">
-        <v>0</v>
-      </c>
-      <c r="E24" t="n">
-        <v>0</v>
-      </c>
-      <c r="F24" t="n">
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
         <v>9</v>
       </c>
       <c r="G24" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
-      <c r="B25" t="n">
+      <c r="B25">
         <v>12</v>
       </c>
-      <c r="C25" t="n">
-        <v>0</v>
-      </c>
-      <c r="D25" t="n">
-        <v>0</v>
-      </c>
-      <c r="E25" t="n">
-        <v>0</v>
-      </c>
-      <c r="F25" t="n">
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
         <v>12</v>
       </c>
       <c r="G25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
-      <c r="B26" t="n">
+      <c r="B26">
         <v>9</v>
       </c>
-      <c r="C26" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" t="n">
-        <v>0</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0</v>
-      </c>
-      <c r="F26" t="n">
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
         <v>9</v>
       </c>
       <c r="G26" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
-      <c r="B27" t="n">
+      <c r="B27">
         <v>12</v>
       </c>
-      <c r="C27" t="n">
+      <c r="C27">
         <v>2</v>
       </c>
-      <c r="D27" t="n">
-        <v>0</v>
-      </c>
-      <c r="E27" t="n">
-        <v>0</v>
-      </c>
-      <c r="F27" t="n">
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
         <v>14</v>
       </c>
       <c r="G27" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>36</v>
       </c>
-      <c r="B28" t="n">
+      <c r="B28">
         <v>12</v>
       </c>
-      <c r="C28" t="n">
+      <c r="C28">
         <v>2</v>
       </c>
-      <c r="D28" t="n">
-        <v>0</v>
-      </c>
-      <c r="E28" t="n">
-        <v>0</v>
-      </c>
-      <c r="F28" t="n">
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
         <v>14</v>
       </c>
       <c r="G28" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:7">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>37</v>
       </c>
-      <c r="B29" t="n">
+      <c r="B29">
         <v>24</v>
       </c>
-      <c r="C29" t="n">
-        <v>0</v>
-      </c>
-      <c r="D29" t="n">
-        <v>0</v>
-      </c>
-      <c r="E29" t="n">
-        <v>0</v>
-      </c>
-      <c r="F29" t="n">
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
         <v>24</v>
       </c>
       <c r="G29" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>39</v>
       </c>
-      <c r="B30" t="n">
+      <c r="B30">
         <v>24</v>
       </c>
-      <c r="C30" t="n">
-        <v>0</v>
-      </c>
-      <c r="D30" t="n">
-        <v>0</v>
-      </c>
-      <c r="E30" t="n">
-        <v>0</v>
-      </c>
-      <c r="F30" t="n">
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>0</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
         <v>24</v>
       </c>
       <c r="G30" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:7">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>40</v>
       </c>
-      <c r="B31" t="n">
+      <c r="B31">
         <v>24</v>
       </c>
-      <c r="C31" t="n">
-        <v>0</v>
-      </c>
-      <c r="D31" t="n">
-        <v>0</v>
-      </c>
-      <c r="E31" t="n">
-        <v>0</v>
-      </c>
-      <c r="F31" t="n">
+      <c r="C31">
+        <v>0</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
         <v>24</v>
       </c>
       <c r="G31" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:7">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>41</v>
       </c>
-      <c r="B32" t="n">
+      <c r="B32">
         <v>24</v>
       </c>
-      <c r="C32" t="n">
-        <v>0</v>
-      </c>
-      <c r="D32" t="n">
-        <v>0</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0</v>
-      </c>
-      <c r="F32" t="n">
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
         <v>24</v>
       </c>
       <c r="G32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="33" spans="1:7">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>42</v>
       </c>
-      <c r="B33" t="n">
+      <c r="B33">
         <v>24</v>
       </c>
-      <c r="C33" t="n">
-        <v>0</v>
-      </c>
-      <c r="D33" t="n">
-        <v>0</v>
-      </c>
-      <c r="E33" t="n">
-        <v>0</v>
-      </c>
-      <c r="F33" t="n">
+      <c r="C33">
+        <v>0</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
         <v>24</v>
       </c>
       <c r="G33" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>43</v>
       </c>
-      <c r="B34" t="n">
+      <c r="B34">
         <v>21</v>
       </c>
-      <c r="C34" t="n">
-        <v>0</v>
-      </c>
-      <c r="D34" t="n">
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
         <v>4</v>
       </c>
-      <c r="E34" t="n">
-        <v>0</v>
-      </c>
-      <c r="F34" t="n">
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
         <v>25</v>
       </c>
       <c r="G34" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>44</v>
       </c>
-      <c r="B35" t="n">
+      <c r="B35">
         <v>21</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35">
         <v>2</v>
       </c>
-      <c r="D35" t="n">
-        <v>0</v>
-      </c>
-      <c r="E35" t="n">
-        <v>0</v>
-      </c>
-      <c r="F35" t="n">
+      <c r="D35">
+        <v>0</v>
+      </c>
+      <c r="E35">
+        <v>0</v>
+      </c>
+      <c r="F35">
         <v>23</v>
       </c>
       <c r="G35" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>45</v>
       </c>
-      <c r="B36" t="n">
+      <c r="B36">
         <v>24</v>
       </c>
-      <c r="C36" t="n">
-        <v>0</v>
-      </c>
-      <c r="D36" t="n">
-        <v>0</v>
-      </c>
-      <c r="E36" t="n">
-        <v>0</v>
-      </c>
-      <c r="F36" t="n">
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
         <v>24</v>
       </c>
       <c r="G36" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B37" t="n">
+      <c r="B37">
         <v>24</v>
       </c>
-      <c r="C37" t="n">
-        <v>0</v>
-      </c>
-      <c r="D37" t="n">
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
         <v>2</v>
       </c>
-      <c r="E37" t="n">
-        <v>0</v>
-      </c>
-      <c r="F37" t="n">
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
         <v>26</v>
       </c>
       <c r="G37" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>47</v>
       </c>
-      <c r="B38" t="n">
+      <c r="B38">
         <v>27</v>
       </c>
-      <c r="C38" t="n">
-        <v>0</v>
-      </c>
-      <c r="D38" t="n">
-        <v>0</v>
-      </c>
-      <c r="E38" t="n">
-        <v>0</v>
-      </c>
-      <c r="F38" t="n">
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>0</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
         <v>27</v>
       </c>
       <c r="G38" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>49</v>
       </c>
-      <c r="B39" t="n">
+      <c r="B39">
         <v>27</v>
       </c>
-      <c r="C39" t="n">
-        <v>0</v>
-      </c>
-      <c r="D39" t="n">
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
         <v>2</v>
       </c>
-      <c r="E39" t="n">
-        <v>0</v>
-      </c>
-      <c r="F39" t="n">
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
         <v>29</v>
       </c>
       <c r="G39" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>50</v>
       </c>
-      <c r="B40" t="n">
+      <c r="B40">
         <v>27</v>
       </c>
-      <c r="C40" t="n">
-        <v>0</v>
-      </c>
-      <c r="D40" t="n">
-        <v>0</v>
-      </c>
-      <c r="E40" t="n">
-        <v>0</v>
-      </c>
-      <c r="F40" t="n">
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
         <v>27</v>
       </c>
       <c r="G40" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="41" spans="1:7">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>51</v>
       </c>
-      <c r="B41" t="n">
+      <c r="B41">
         <v>27</v>
       </c>
-      <c r="C41" t="n">
-        <v>0</v>
-      </c>
-      <c r="D41" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" t="n">
-        <v>0</v>
-      </c>
-      <c r="F41" t="n">
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
         <v>27</v>
       </c>
       <c r="G41" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>52</v>
       </c>
-      <c r="B42" t="n">
+      <c r="B42">
         <v>27</v>
       </c>
-      <c r="C42" t="n">
-        <v>0</v>
-      </c>
-      <c r="D42" t="n">
-        <v>0</v>
-      </c>
-      <c r="E42" t="n">
-        <v>0</v>
-      </c>
-      <c r="F42" t="n">
+      <c r="C42">
+        <v>0</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
         <v>27</v>
       </c>
       <c r="G42" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>53</v>
       </c>
-      <c r="B43" t="n">
+      <c r="B43">
         <v>27</v>
       </c>
-      <c r="C43" t="n">
-        <v>0</v>
-      </c>
-      <c r="D43" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" t="n">
-        <v>0</v>
-      </c>
-      <c r="F43" t="n">
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+      <c r="F43">
         <v>27</v>
       </c>
       <c r="G43" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>54</v>
       </c>
-      <c r="B44" t="n">
+      <c r="B44">
         <v>27</v>
       </c>
-      <c r="C44" t="n">
-        <v>0</v>
-      </c>
-      <c r="D44" t="n">
-        <v>0</v>
-      </c>
-      <c r="E44" t="n">
-        <v>0</v>
-      </c>
-      <c r="F44" t="n">
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+      <c r="F44">
         <v>27</v>
       </c>
       <c r="G44" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>55</v>
       </c>
-      <c r="B45" t="n">
+      <c r="B45">
         <v>27</v>
       </c>
-      <c r="C45" t="n">
-        <v>0</v>
-      </c>
-      <c r="D45" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" t="n">
-        <v>0</v>
-      </c>
-      <c r="F45" t="n">
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
         <v>27</v>
       </c>
       <c r="G45" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>56</v>
       </c>
-      <c r="B46" t="n">
+      <c r="B46">
         <v>27</v>
       </c>
-      <c r="C46" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" t="n">
-        <v>0</v>
-      </c>
-      <c r="E46" t="n">
-        <v>0</v>
-      </c>
-      <c r="F46" t="n">
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
         <v>27</v>
       </c>
       <c r="G46" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>57</v>
       </c>
-      <c r="B47" t="n">
+      <c r="B47">
         <v>39</v>
       </c>
-      <c r="C47" t="n">
-        <v>0</v>
-      </c>
-      <c r="D47" t="n">
-        <v>0</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0</v>
-      </c>
-      <c r="F47" t="n">
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
         <v>39</v>
       </c>
       <c r="G47" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>59</v>
       </c>
-      <c r="B48" t="n">
+      <c r="B48">
         <v>36</v>
       </c>
-      <c r="C48" t="n">
-        <v>0</v>
-      </c>
-      <c r="D48" t="n">
-        <v>0</v>
-      </c>
-      <c r="E48" t="n">
-        <v>0</v>
-      </c>
-      <c r="F48" t="n">
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
         <v>36</v>
       </c>
       <c r="G48" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>60</v>
       </c>
-      <c r="B49" t="n">
+      <c r="B49">
         <v>36</v>
       </c>
-      <c r="C49" t="n">
-        <v>0</v>
-      </c>
-      <c r="D49" t="n">
-        <v>0</v>
-      </c>
-      <c r="E49" t="n">
-        <v>0</v>
-      </c>
-      <c r="F49" t="n">
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
         <v>36</v>
       </c>
       <c r="G49" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>61</v>
       </c>
-      <c r="B50" t="n">
+      <c r="B50">
         <v>33</v>
       </c>
-      <c r="C50" t="n">
-        <v>0</v>
-      </c>
-      <c r="D50" t="n">
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
         <v>2</v>
       </c>
-      <c r="E50" t="n">
-        <v>0</v>
-      </c>
-      <c r="F50" t="n">
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
         <v>35</v>
       </c>
       <c r="G50" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>62</v>
       </c>
-      <c r="B51" t="n">
+      <c r="B51">
         <v>36</v>
       </c>
-      <c r="C51" t="n">
-        <v>0</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
-      </c>
-      <c r="F51" t="n">
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
         <v>36</v>
       </c>
       <c r="G51" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>63</v>
       </c>
-      <c r="B52" t="n">
+      <c r="B52">
         <v>45</v>
       </c>
-      <c r="C52" t="n">
+      <c r="C52">
         <v>2</v>
       </c>
-      <c r="D52" t="n">
-        <v>0</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
-      </c>
-      <c r="F52" t="n">
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
         <v>47</v>
       </c>
       <c r="G52" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>64</v>
       </c>
-      <c r="B53" t="n">
+      <c r="B53">
         <v>36</v>
       </c>
-      <c r="C53" t="n">
-        <v>0</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
-      </c>
-      <c r="F53" t="n">
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
         <v>36</v>
       </c>
       <c r="G53" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="54" spans="1:7">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>65</v>
       </c>
-      <c r="B54" t="n">
+      <c r="B54">
         <v>45</v>
       </c>
-      <c r="C54" t="n">
-        <v>0</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
-      </c>
-      <c r="F54" t="n">
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
         <v>45</v>
       </c>
       <c r="G54" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
-      <c r="A55" t="s">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A55" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B55" t="n">
-        <v>42</v>
-      </c>
-      <c r="C55" t="n">
-        <v>2</v>
-      </c>
-      <c r="D55" t="n">
-        <v>0</v>
-      </c>
-      <c r="E55" t="n">
-        <v>0</v>
-      </c>
-      <c r="F55" t="n">
-        <v>44</v>
-      </c>
-      <c r="G55" t="s">
+      <c r="B55" s="2">
+        <v>36</v>
+      </c>
+      <c r="C55" s="2">
+        <v>0</v>
+      </c>
+      <c r="D55" s="2">
+        <v>0</v>
+      </c>
+      <c r="E55" s="2">
+        <v>0</v>
+      </c>
+      <c r="F55" s="2">
+        <v>36</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>58</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>